<commit_message>
Created methods what assign appropriate values from call off's order to confirmed order's part, calculates quantity for remaining part and changes postfixes in order number
</commit_message>
<xml_diff>
--- a/data/output2.xlsx
+++ b/data/output2.xlsx
@@ -599,14 +599,14 @@
         <v>433</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>44137</v>
+        <v>44150</v>
       </c>
       <c r="N2" t="n">
         <v>2178</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>to be called off</t>
+          <t>confirmed</t>
         </is>
       </c>
       <c r="P2" s="2" t="n">
@@ -614,8 +614,12 @@
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
+      <c r="S2" s="2" t="n">
+        <v>44150</v>
+      </c>
+      <c r="T2" t="n">
+        <v>433</v>
+      </c>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
@@ -636,7 +640,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2437589/8</t>
+          <t>2437589/9</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
@@ -664,10 +668,10 @@
         <v>811122</v>
       </c>
       <c r="K3" t="n">
-        <v>433</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>433</v>
+        <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
         <v>44137</v>

</xml_diff>